<commit_message>
Feat : Added Create Operation from CRUD OP
</commit_message>
<xml_diff>
--- a/Testdata/magnustestdata.xlsx
+++ b/Testdata/magnustestdata.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" r:id="rId1"/>
+    <sheet name="empdata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -37,13 +38,58 @@
   </si>
   <si>
     <t>Welcome to JALA Academy</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>Klatur</t>
+  </si>
+  <si>
+    <t>kiran@gmail.com</t>
+  </si>
+  <si>
+    <t>9955886495</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>update</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Record deleted successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee details updated successfully </t>
+  </si>
+  <si>
+    <t>Employee details saved successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +102,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -96,10 +150,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -117,8 +172,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -399,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,6 +480,7 @@
     <col min="1" max="1" width="31.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="66.140625" customWidth="1"/>
+    <col min="4" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -506,4 +579,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="8" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update : added CRUD Package
</commit_message>
<xml_diff>
--- a/Testdata/magnustestdata.xlsx
+++ b/Testdata/magnustestdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -83,6 +83,18 @@
   </si>
   <si>
     <t>Employee details saved successfully</t>
+  </si>
+  <si>
+    <t>sameer</t>
+  </si>
+  <si>
+    <t>sajid</t>
+  </si>
+  <si>
+    <t>sameer@gmail.com</t>
+  </si>
+  <si>
+    <t>9865486245</t>
   </si>
 </sst>
 </file>
@@ -154,7 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -188,6 +200,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -585,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,10 +662,18 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="E3" s="12"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -790,8 +812,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update : added extend report
</commit_message>
<xml_diff>
--- a/Testdata/magnustestdata.xlsx
+++ b/Testdata/magnustestdata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">username </t>
   </si>
@@ -95,6 +95,18 @@
   </si>
   <si>
     <t>9865486245</t>
+  </si>
+  <si>
+    <t>raj</t>
+  </si>
+  <si>
+    <t>rajiv</t>
+  </si>
+  <si>
+    <t>raj@hot.com</t>
+  </si>
+  <si>
+    <t>8564689656</t>
   </si>
 </sst>
 </file>
@@ -674,16 +686,26 @@
       <c r="D3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -813,8 +835,9 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>